<commit_message>
Added data redcution for Loop.
</commit_message>
<xml_diff>
--- a/data/data_1.xlsx
+++ b/data/data_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanscastorp/Dropbox/Thing/MIT/nano fluids/model_python/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanscastorp/Colloid-model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919AEBA1-DB37-AA4D-B5D6-F0E6ACD87BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902648AE-93B8-7B41-A653-D27B365D8CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="460" windowWidth="22380" windowHeight="15960" xr2:uid="{F1969B3A-D447-2245-9C7E-19D3CC58A2E2}"/>
+    <workbookView xWindow="4460" yWindow="500" windowWidth="22380" windowHeight="15960" activeTab="1" xr2:uid="{F1969B3A-D447-2245-9C7E-19D3CC58A2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="nanoparticle" sheetId="1" r:id="rId1"/>
@@ -3676,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF4C50A-A313-F546-AE86-448D291CD1A2}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -4743,8 +4743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1512B1-73EC-AC44-9E15-5BAA90EC537C}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5027,6 +5027,15 @@
       </c>
       <c r="J7">
         <v>2.14E-4</v>
+      </c>
+      <c r="K7">
+        <v>247.8</v>
+      </c>
+      <c r="L7">
+        <v>140</v>
+      </c>
+      <c r="M7">
+        <v>2.4139999999999999E-5</v>
       </c>
       <c r="N7">
         <v>70</v>

</xml_diff>